<commit_message>
Base station pin mappings rust file
</commit_message>
<xml_diff>
--- a/PSat/Base Station/Base Station Pin Mappings.xlsx
+++ b/PSat/Base Station/Base Station Pin Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\APSS-Reference-PCBs\PSat\Base Station\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272D7B82-BBC8-44FD-A7C6-DD5BE2061F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0AC302-C07B-49A7-BC33-7BA39CFBFADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9600" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Beacon V2.1 Pin Mappings</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>P2.2</t>
+  </si>
+  <si>
+    <t>Display SDA</t>
+  </si>
+  <si>
+    <t>Display SCL</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,6 +565,22 @@
         <v>28</v>
       </c>
     </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>